<commit_message>
Updated Correlation matrix to include sentiment score
</commit_message>
<xml_diff>
--- a/Correlation_Matrix.xlsx
+++ b/Correlation_Matrix.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="23">
   <si>
     <t>movie_title</t>
   </si>
@@ -86,6 +86,9 @@
   <si>
     <t>aspect_ratio</t>
   </si>
+  <si>
+    <t>plot_sentiment</t>
+  </si>
 </sst>
 </file>
 
@@ -116,12 +119,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -180,9 +189,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -560,10 +572,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W23"/>
+  <dimension ref="A1:X24"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -572,75 +584,78 @@
     <col min="2" max="2" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="30">
+    <row r="1" spans="1:24" ht="30">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:24">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -651,67 +666,70 @@
         <v>0.99980438939819605</v>
       </c>
       <c r="D2" s="1">
+        <v>6.5196964343612301E-2</v>
+      </c>
+      <c r="E2" s="1">
         <v>0.99849370918185798</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F2" s="1">
         <v>0.410143670895465</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G2" s="1">
         <v>0.59472588050535102</v>
       </c>
-      <c r="G2" s="1">
+      <c r="H2" s="1">
         <v>-0.25513879164953301</v>
       </c>
-      <c r="H2" s="1">
+      <c r="I2" s="1">
         <v>0.809792888588867</v>
       </c>
-      <c r="I2" s="1">
+      <c r="J2" s="1">
         <v>0.69648494391427695</v>
       </c>
-      <c r="J2" s="1">
+      <c r="K2" s="1">
         <v>-0.10780929601481</v>
       </c>
-      <c r="K2" s="1">
+      <c r="L2" s="1">
         <v>0.78405290692770402</v>
       </c>
-      <c r="L2" s="1">
+      <c r="M2" s="1">
         <v>-6.0427788055856302E-2</v>
       </c>
-      <c r="M2" s="1">
+      <c r="N2" s="1">
         <v>0.82953931281323101</v>
       </c>
-      <c r="N2" s="1">
+      <c r="O2" s="1">
         <v>-5.9284016850549598E-2</v>
       </c>
-      <c r="O2" s="1">
+      <c r="P2" s="1">
         <v>-6.4356048591548498E-3</v>
       </c>
-      <c r="P2" s="1">
+      <c r="Q2" s="1">
         <v>-0.37757899773043102</v>
       </c>
-      <c r="Q2" s="1">
+      <c r="R2" s="1">
         <v>0.13964079269922999</v>
       </c>
-      <c r="R2" s="1">
+      <c r="S2" s="1">
         <v>-0.35900228946907298</v>
       </c>
-      <c r="S2" s="1">
+      <c r="T2" s="1">
         <v>-0.33986937510027498</v>
       </c>
-      <c r="T2" s="1">
+      <c r="U2" s="1">
         <v>0.158547389500029</v>
       </c>
-      <c r="U2" s="1">
+      <c r="V2" s="1">
         <v>0.15663073697514199</v>
       </c>
-      <c r="V2" s="1">
+      <c r="W2" s="1">
         <v>0.36082637349743701</v>
       </c>
-      <c r="W2" s="1">
+      <c r="X2" s="1">
         <v>-1.38913900613486E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:24">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -722,1483 +740,1620 @@
         <v>1</v>
       </c>
       <c r="D3" s="1">
+        <v>6.1913975943279902E-2</v>
+      </c>
+      <c r="E3" s="1">
         <v>0.998710180103205</v>
       </c>
-      <c r="E3" s="1">
+      <c r="F3" s="1">
         <v>0.41065294318670698</v>
       </c>
-      <c r="F3" s="1">
+      <c r="G3" s="1">
         <v>0.59436167100072401</v>
       </c>
-      <c r="G3" s="1">
+      <c r="H3" s="1">
         <v>-0.256214142364867</v>
       </c>
-      <c r="H3" s="1">
+      <c r="I3" s="1">
         <v>0.80922136300374803</v>
       </c>
-      <c r="I3" s="1">
+      <c r="J3" s="1">
         <v>0.69650525113984996</v>
       </c>
-      <c r="J3" s="1">
+      <c r="K3" s="1">
         <v>-0.10786218033837</v>
       </c>
-      <c r="K3" s="1">
+      <c r="L3" s="1">
         <v>0.78445421019792105</v>
       </c>
-      <c r="L3" s="1">
+      <c r="M3" s="1">
         <v>-6.0414778618035798E-2</v>
       </c>
-      <c r="M3" s="1">
+      <c r="N3" s="1">
         <v>0.82931677738246801</v>
       </c>
-      <c r="N3" s="1">
+      <c r="O3" s="1">
         <v>-5.9246892135405203E-2</v>
       </c>
-      <c r="O3" s="1">
+      <c r="P3" s="1">
         <v>-6.4070399287441699E-3</v>
       </c>
-      <c r="P3" s="1">
+      <c r="Q3" s="1">
         <v>-0.37776479910271898</v>
       </c>
-      <c r="Q3" s="1">
+      <c r="R3" s="1">
         <v>0.140383475580452</v>
       </c>
-      <c r="R3" s="1">
+      <c r="S3" s="1">
         <v>-0.35147626159824102</v>
       </c>
-      <c r="S3" s="1">
+      <c r="T3" s="1">
         <v>-0.33121623145919099</v>
       </c>
-      <c r="T3" s="1">
+      <c r="U3" s="1">
         <v>0.160128190714033</v>
       </c>
-      <c r="U3" s="1">
+      <c r="V3" s="1">
         <v>0.15765222565210299</v>
       </c>
-      <c r="V3" s="1">
+      <c r="W3" s="1">
         <v>0.36076580547304299</v>
       </c>
-      <c r="W3" s="1">
+      <c r="X3" s="1">
         <v>-1.34636929694276E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:23">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:24">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="1">
+        <v>6.5196964343612301E-2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>6.1913975943279902E-2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>6.3415061476320395E-2</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2.13165726687107E-2</v>
+      </c>
+      <c r="G4" s="1">
+        <v>-4.0243077519733104E-3</v>
+      </c>
+      <c r="H4" s="1">
+        <v>-1.7035290376341099E-2</v>
+      </c>
+      <c r="I4" s="1">
+        <v>5.8418826423703503E-2</v>
+      </c>
+      <c r="J4" s="1">
+        <v>3.9435637155291803E-2</v>
+      </c>
+      <c r="K4" s="1">
+        <v>-1.8310321048661801E-2</v>
+      </c>
+      <c r="L4" s="1">
+        <v>4.8064604313819703E-2</v>
+      </c>
+      <c r="M4" s="1">
+        <v>7.8799806840581191E-3</v>
+      </c>
+      <c r="N4" s="1">
+        <v>4.5054659352377797E-2</v>
+      </c>
+      <c r="O4" s="1">
+        <v>3.9442973294892504E-3</v>
+      </c>
+      <c r="P4" s="1">
+        <v>2.9092633138568101E-2</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>-5.89000038995382E-2</v>
+      </c>
+      <c r="R4" s="1">
+        <v>4.2543278785014897E-2</v>
+      </c>
+      <c r="S4" s="1">
+        <v>-3.4044314085956297E-2</v>
+      </c>
+      <c r="T4" s="1">
+        <v>-4.0034757956118897E-2</v>
+      </c>
+      <c r="U4" s="1">
+        <v>1.1101529625722599E-2</v>
+      </c>
+      <c r="V4" s="1">
+        <v>-1.8688684323293701E-2</v>
+      </c>
+      <c r="W4" s="1">
+        <v>-7.9142521001483706E-3</v>
+      </c>
+      <c r="X4" s="1">
+        <v>-7.0963342595646199E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24">
+      <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B5" s="1">
         <v>0.99849370918185798</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C5" s="1">
         <v>0.998710180103205</v>
       </c>
-      <c r="D4" s="1">
-        <v>1</v>
-      </c>
-      <c r="E4" s="1">
+      <c r="D5" s="1">
+        <v>6.3415061476320395E-2</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1">
         <v>0.41110223661345402</v>
       </c>
-      <c r="F4" s="1">
+      <c r="G5" s="1">
         <v>0.59165715197386404</v>
       </c>
-      <c r="G4" s="1">
+      <c r="H5" s="1">
         <v>-0.25061800966390102</v>
       </c>
-      <c r="H4" s="1">
+      <c r="I5" s="1">
         <v>0.79712224846328095</v>
       </c>
-      <c r="I4" s="1">
+      <c r="J5" s="1">
         <v>0.68521437708224897</v>
       </c>
-      <c r="J4" s="1">
+      <c r="K5" s="1">
         <v>-0.106102134696655</v>
       </c>
-      <c r="K4" s="1">
+      <c r="L5" s="1">
         <v>0.77813073130227195</v>
       </c>
-      <c r="L4" s="1">
+      <c r="M5" s="1">
         <v>-5.7796061324969901E-2</v>
       </c>
-      <c r="M4" s="1">
+      <c r="N5" s="1">
         <v>0.824898287043488</v>
       </c>
-      <c r="N4" s="1">
+      <c r="O5" s="1">
         <v>-5.7649057638550202E-2</v>
       </c>
-      <c r="O4" s="1">
+      <c r="P5" s="1">
         <v>1.0192436571006399E-2</v>
       </c>
-      <c r="P4" s="1">
+      <c r="Q5" s="1">
         <v>-0.37222931181248903</v>
       </c>
-      <c r="Q4" s="1">
+      <c r="R5" s="1">
         <v>0.14443773167414201</v>
       </c>
-      <c r="R4" s="1">
+      <c r="S5" s="1">
         <v>-0.34969712063187403</v>
       </c>
-      <c r="S4" s="1">
+      <c r="T5" s="1">
         <v>-0.33126226376010198</v>
       </c>
-      <c r="T4" s="1">
+      <c r="U5" s="1">
         <v>0.15579318259889099</v>
       </c>
-      <c r="U4" s="1">
+      <c r="V5" s="1">
         <v>0.15176570459345301</v>
       </c>
-      <c r="V4" s="1">
+      <c r="W5" s="1">
         <v>0.36388318087433702</v>
       </c>
-      <c r="W4" s="1">
+      <c r="X5" s="1">
         <v>-2.48133817072945E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:23">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:24">
+      <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B6" s="1">
         <v>0.410143670895465</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C6" s="1">
         <v>0.41065294318670698</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D6" s="1">
+        <v>2.13165726687107E-2</v>
+      </c>
+      <c r="E6" s="1">
         <v>0.41110223661345402</v>
       </c>
-      <c r="E5" s="1">
-        <v>1</v>
-      </c>
-      <c r="F5" s="1">
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1">
         <v>0.29133992078107601</v>
       </c>
-      <c r="G5" s="1">
+      <c r="H6" s="1">
         <v>-8.3211999826188696E-2</v>
       </c>
-      <c r="H5" s="1">
+      <c r="I6" s="1">
         <v>0.34916475376501799</v>
       </c>
-      <c r="I5" s="1">
+      <c r="J6" s="1">
         <v>0.33438621144262198</v>
       </c>
-      <c r="J5" s="1">
+      <c r="K6" s="1">
         <v>-4.5801475608615097E-2</v>
       </c>
-      <c r="K5" s="1">
+      <c r="L6" s="1">
         <v>0.342485083484313</v>
       </c>
-      <c r="L5" s="1">
+      <c r="M6" s="1">
         <v>-1.89899379176257E-2</v>
       </c>
-      <c r="M5" s="1">
+      <c r="N6" s="1">
         <v>0.37065066700242599</v>
       </c>
-      <c r="N5" s="1">
+      <c r="O6" s="1">
         <v>-1.9336857556304401E-2</v>
       </c>
-      <c r="O5" s="1">
+      <c r="P6" s="1">
         <v>-2.4707453693601001E-3</v>
       </c>
-      <c r="P5" s="1">
+      <c r="Q6" s="1">
         <v>-0.204306532318446</v>
       </c>
-      <c r="Q5" s="1">
+      <c r="R6" s="1">
         <v>7.6023292156156302E-2</v>
       </c>
-      <c r="R5" s="1">
+      <c r="S6" s="1">
         <v>-0.160096799255316</v>
       </c>
-      <c r="S5" s="1">
+      <c r="T6" s="1">
         <v>-0.153085545779267</v>
       </c>
-      <c r="T5" s="1">
+      <c r="U6" s="1">
         <v>5.4749769816534698E-2</v>
       </c>
-      <c r="U5" s="1">
+      <c r="V6" s="1">
         <v>4.26502746904645E-2</v>
       </c>
-      <c r="V5" s="1">
+      <c r="W6" s="1">
         <v>0.167463118225393</v>
       </c>
-      <c r="W5" s="1">
+      <c r="X6" s="1">
         <v>-2.80160139628737E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:23">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:24">
+      <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B7" s="1">
         <v>0.59472588050535102</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C7" s="1">
         <v>0.59436167100072401</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D7" s="1">
+        <v>-4.0243077519733104E-3</v>
+      </c>
+      <c r="E7" s="1">
         <v>0.59165715197386404</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F7" s="1">
         <v>0.29133992078107601</v>
       </c>
-      <c r="F6" s="1">
-        <v>1</v>
-      </c>
-      <c r="G6" s="1">
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1">
         <v>-0.133643644174534</v>
       </c>
-      <c r="H6" s="1">
+      <c r="I7" s="1">
         <v>0.458803200314779</v>
       </c>
-      <c r="I6" s="1">
+      <c r="J7" s="1">
         <v>0.43574097090228497</v>
       </c>
-      <c r="J6" s="1">
+      <c r="K7" s="1">
         <v>-0.10795233114173899</v>
       </c>
-      <c r="K6" s="1">
+      <c r="L7" s="1">
         <v>0.49685913737923698</v>
       </c>
-      <c r="L6" s="1">
+      <c r="M7" s="1">
         <v>-6.2035063952588398E-2</v>
       </c>
-      <c r="M6" s="1">
+      <c r="N7" s="1">
         <v>0.49834246183970299</v>
       </c>
-      <c r="N6" s="1">
+      <c r="O7" s="1">
         <v>-6.5784057174292601E-2</v>
       </c>
-      <c r="O6" s="1">
+      <c r="P7" s="1">
         <v>2.6804991343021001E-2</v>
       </c>
-      <c r="P6" s="1">
+      <c r="Q7" s="1">
         <v>-0.25337149820265797</v>
       </c>
-      <c r="Q6" s="1">
+      <c r="R7" s="1">
         <v>8.8547129555941795E-2</v>
       </c>
-      <c r="R6" s="1">
+      <c r="S7" s="1">
         <v>-0.25328117586416798</v>
       </c>
-      <c r="S6" s="1">
+      <c r="T7" s="1">
         <v>-0.23454979796974099</v>
       </c>
-      <c r="T6" s="1">
+      <c r="U7" s="1">
         <v>9.78272645040488E-2</v>
       </c>
-      <c r="U6" s="1">
+      <c r="V7" s="1">
         <v>9.66665551086099E-2</v>
       </c>
-      <c r="V6" s="1">
+      <c r="W7" s="1">
         <v>0.35248858014956302</v>
       </c>
-      <c r="W6" s="1">
+      <c r="X7" s="1">
         <v>1.27596430203949E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:23">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="1:24">
+      <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B8" s="1">
         <v>-0.25513879164953301</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C8" s="1">
         <v>-0.256214142364867</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D8" s="1">
+        <v>-1.7035290376341099E-2</v>
+      </c>
+      <c r="E8" s="1">
         <v>-0.25061800966390102</v>
       </c>
-      <c r="E7" s="1">
+      <c r="F8" s="1">
         <v>-8.3211999826188696E-2</v>
       </c>
-      <c r="F7" s="1">
+      <c r="G8" s="1">
         <v>-0.133643644174534</v>
       </c>
-      <c r="G7" s="1">
-        <v>1</v>
-      </c>
-      <c r="H7" s="1">
+      <c r="H8" s="1">
+        <v>1</v>
+      </c>
+      <c r="I8" s="1">
         <v>-0.313928833540977</v>
       </c>
-      <c r="I7" s="1">
+      <c r="J8" s="1">
         <v>-0.19368254162288301</v>
       </c>
-      <c r="J7" s="1">
+      <c r="K8" s="1">
         <v>3.8954237135927397E-2</v>
       </c>
-      <c r="K7" s="1">
+      <c r="L8" s="1">
         <v>-0.20311823871658999</v>
       </c>
-      <c r="L7" s="1">
+      <c r="M8" s="1">
         <v>-2.4345175331035199E-3</v>
       </c>
-      <c r="M7" s="1">
+      <c r="N8" s="1">
         <v>-0.22966969875881099</v>
       </c>
-      <c r="N7" s="1">
+      <c r="O8" s="1">
         <v>5.2996348825765302E-3</v>
       </c>
-      <c r="O7" s="1">
+      <c r="P8" s="1">
         <v>0.27997741363661999</v>
       </c>
-      <c r="P7" s="1">
+      <c r="Q8" s="1">
         <v>0.28744392203068803</v>
       </c>
-      <c r="Q7" s="1">
+      <c r="R8" s="1">
         <v>0.26762153705583802</v>
       </c>
-      <c r="R7" s="1">
+      <c r="S8" s="1">
         <v>0.17959151254904701</v>
       </c>
-      <c r="S7" s="1">
+      <c r="T8" s="1">
         <v>0.17529322024326099</v>
       </c>
-      <c r="T7" s="1">
+      <c r="U8" s="1">
         <v>8.2227941978073801E-2</v>
       </c>
-      <c r="U7" s="1">
+      <c r="V8" s="1">
         <v>7.0725267050235796E-2</v>
       </c>
-      <c r="V7" s="1">
+      <c r="W8" s="1">
         <v>-4.9181399633654699E-2</v>
       </c>
-      <c r="W7" s="1">
+      <c r="X8" s="1">
         <v>-0.11376401354828899</v>
       </c>
     </row>
-    <row r="8" spans="1:23">
-      <c r="A8" s="1" t="s">
+    <row r="9" spans="1:24">
+      <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B9" s="1">
         <v>0.809792888588867</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C9" s="1">
         <v>0.80922136300374803</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D9" s="1">
+        <v>5.8418826423703503E-2</v>
+      </c>
+      <c r="E9" s="1">
         <v>0.79712224846328095</v>
       </c>
-      <c r="E8" s="1">
+      <c r="F9" s="1">
         <v>0.34916475376501799</v>
       </c>
-      <c r="F8" s="1">
+      <c r="G9" s="1">
         <v>0.458803200314779</v>
       </c>
-      <c r="G8" s="1">
+      <c r="H9" s="1">
         <v>-0.313928833540977</v>
       </c>
-      <c r="H8" s="1">
-        <v>1</v>
-      </c>
-      <c r="I8" s="1">
+      <c r="I9" s="1">
+        <v>1</v>
+      </c>
+      <c r="J9" s="1">
         <v>0.65537193107733505</v>
       </c>
-      <c r="J8" s="1">
+      <c r="K9" s="1">
         <v>-8.7755314017052694E-2</v>
       </c>
-      <c r="K8" s="1">
+      <c r="L9" s="1">
         <v>0.69426305566160595</v>
       </c>
-      <c r="L8" s="1">
+      <c r="M9" s="1">
         <v>-4.5622654964447701E-2</v>
       </c>
-      <c r="M8" s="1">
+      <c r="N9" s="1">
         <v>0.716496238438313</v>
       </c>
-      <c r="N8" s="1">
+      <c r="O9" s="1">
         <v>-4.4383525496576502E-2</v>
       </c>
-      <c r="O8" s="1">
+      <c r="P9" s="1">
         <v>-0.137694814632288</v>
       </c>
-      <c r="P8" s="1">
+      <c r="Q9" s="1">
         <v>-0.405744291142562</v>
       </c>
-      <c r="Q8" s="1">
+      <c r="R9" s="1">
         <v>-1.5969107993542501E-3</v>
       </c>
-      <c r="R8" s="1">
+      <c r="S9" s="1">
         <v>-0.25764650010722501</v>
       </c>
-      <c r="S8" s="1">
+      <c r="T9" s="1">
         <v>-0.232515081609737</v>
       </c>
-      <c r="T8" s="1">
+      <c r="U9" s="1">
         <v>0.159663790236064</v>
       </c>
-      <c r="U8" s="1">
+      <c r="V9" s="1">
         <v>0.180142957024571</v>
       </c>
-      <c r="V8" s="1">
+      <c r="W9" s="1">
         <v>0.30193287043511802</v>
       </c>
-      <c r="W8" s="1">
+      <c r="X9" s="1">
         <v>1.15459971934405E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:23">
-      <c r="A9" s="1" t="s">
+    <row r="10" spans="1:24">
+      <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B10" s="1">
         <v>0.69648494391427695</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C10" s="1">
         <v>0.69650525113984996</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D10" s="1">
+        <v>3.9435637155291803E-2</v>
+      </c>
+      <c r="E10" s="1">
         <v>0.68521437708224897</v>
       </c>
-      <c r="E9" s="1">
+      <c r="F10" s="1">
         <v>0.33438621144262198</v>
       </c>
-      <c r="F9" s="1">
+      <c r="G10" s="1">
         <v>0.43574097090228497</v>
       </c>
-      <c r="G9" s="1">
+      <c r="H10" s="1">
         <v>-0.19368254162288301</v>
       </c>
-      <c r="H9" s="1">
+      <c r="I10" s="1">
         <v>0.65537193107733505</v>
       </c>
-      <c r="I9" s="1">
-        <v>1</v>
-      </c>
-      <c r="J9" s="1">
+      <c r="J10" s="1">
+        <v>1</v>
+      </c>
+      <c r="K10" s="1">
         <v>-0.121173118484641</v>
       </c>
-      <c r="K9" s="1">
+      <c r="L10" s="1">
         <v>0.72984029462341105</v>
       </c>
-      <c r="L9" s="1">
+      <c r="M10" s="1">
         <v>-7.0223322368931806E-2</v>
       </c>
-      <c r="M9" s="1">
+      <c r="N10" s="1">
         <v>0.68085225192023602</v>
       </c>
-      <c r="N9" s="1">
+      <c r="O10" s="1">
         <v>-5.7117563177665198E-2</v>
       </c>
-      <c r="O9" s="1">
+      <c r="P10" s="1">
         <v>-6.55828885203881E-2</v>
       </c>
-      <c r="P9" s="1">
+      <c r="Q10" s="1">
         <v>-0.32236566895984797</v>
       </c>
-      <c r="Q9" s="1">
+      <c r="R10" s="1">
         <v>7.5053026801822603E-2</v>
       </c>
-      <c r="R9" s="1">
+      <c r="S10" s="1">
         <v>-0.19581622016279601</v>
       </c>
-      <c r="S9" s="1">
+      <c r="T10" s="1">
         <v>-0.163888398594911</v>
       </c>
-      <c r="T9" s="1">
+      <c r="U10" s="1">
         <v>0.221129605573503</v>
       </c>
-      <c r="U9" s="1">
+      <c r="V10" s="1">
         <v>0.20519369984307501</v>
       </c>
-      <c r="V9" s="1">
+      <c r="W10" s="1">
         <v>0.30519050901529099</v>
       </c>
-      <c r="W9" s="1">
+      <c r="X10" s="1">
         <v>1.91520432036506E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:23">
-      <c r="A10" s="1" t="s">
+    <row r="11" spans="1:24">
+      <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B11" s="1">
         <v>-0.10780929601481</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C11" s="1">
         <v>-0.10786218033837</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D11" s="1">
+        <v>-1.8310321048661801E-2</v>
+      </c>
+      <c r="E11" s="1">
         <v>-0.106102134696655</v>
       </c>
-      <c r="E10" s="1">
+      <c r="F11" s="1">
         <v>-4.5801475608615097E-2</v>
       </c>
-      <c r="F10" s="1">
+      <c r="G11" s="1">
         <v>-0.10795233114173899</v>
       </c>
-      <c r="G10" s="1">
+      <c r="H11" s="1">
         <v>3.8954237135927397E-2</v>
       </c>
-      <c r="H10" s="1">
+      <c r="I11" s="1">
         <v>-8.7755314017052694E-2</v>
       </c>
-      <c r="I10" s="1">
+      <c r="J11" s="1">
         <v>-0.121173118484641</v>
       </c>
-      <c r="J10" s="1">
-        <v>1</v>
-      </c>
-      <c r="K10" s="1">
+      <c r="K11" s="1">
+        <v>1</v>
+      </c>
+      <c r="L11" s="1">
         <v>-8.8354463526561899E-2</v>
       </c>
-      <c r="L10" s="1">
+      <c r="M11" s="1">
         <v>2.3054050853716999E-2</v>
       </c>
-      <c r="M10" s="1">
+      <c r="N11" s="1">
         <v>-0.10966046937912299</v>
       </c>
-      <c r="N10" s="1">
+      <c r="O11" s="1">
         <v>3.91858113923442E-2</v>
       </c>
-      <c r="O10" s="1">
+      <c r="P11" s="1">
         <v>-1.43555239103151E-2</v>
       </c>
-      <c r="P10" s="1">
+      <c r="Q11" s="1">
         <v>9.6562390623278302E-2</v>
       </c>
-      <c r="Q10" s="1">
+      <c r="R11" s="1">
         <v>-1.8039308090925001E-2</v>
       </c>
-      <c r="R10" s="1">
+      <c r="S11" s="1">
         <v>4.3301105885510199E-2</v>
       </c>
-      <c r="S10" s="1">
+      <c r="T11" s="1">
         <v>3.1900159353646297E-2</v>
       </c>
-      <c r="T10" s="1">
+      <c r="U11" s="1">
         <v>-2.88341948922398E-2</v>
       </c>
-      <c r="U10" s="1">
+      <c r="V11" s="1">
         <v>-3.2350507379077902E-2</v>
       </c>
-      <c r="V10" s="1">
+      <c r="W11" s="1">
         <v>-5.7516400188989097E-2</v>
       </c>
-      <c r="W10" s="1">
+      <c r="X11" s="1">
         <v>-1.39286712044361E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:23">
-      <c r="A11" s="1" t="s">
+    <row r="12" spans="1:24">
+      <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B12" s="1">
         <v>0.78405290692770402</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C12" s="1">
         <v>0.78445421019792105</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D12" s="1">
+        <v>4.8064604313819703E-2</v>
+      </c>
+      <c r="E12" s="1">
         <v>0.77813073130227195</v>
       </c>
-      <c r="E11" s="1">
+      <c r="F12" s="1">
         <v>0.342485083484313</v>
       </c>
-      <c r="F11" s="1">
+      <c r="G12" s="1">
         <v>0.49685913737923698</v>
       </c>
-      <c r="G11" s="1">
+      <c r="H12" s="1">
         <v>-0.20311823871658999</v>
       </c>
-      <c r="H11" s="1">
+      <c r="I12" s="1">
         <v>0.69426305566160595</v>
       </c>
-      <c r="I11" s="1">
+      <c r="J12" s="1">
         <v>0.72984029462341105</v>
       </c>
-      <c r="J11" s="1">
+      <c r="K12" s="1">
         <v>-8.8354463526561899E-2</v>
       </c>
-      <c r="K11" s="1">
-        <v>1</v>
-      </c>
-      <c r="L11" s="1">
+      <c r="L12" s="1">
+        <v>1</v>
+      </c>
+      <c r="M12" s="1">
         <v>-7.2841808258598595E-2</v>
       </c>
-      <c r="M11" s="1">
+      <c r="N12" s="1">
         <v>0.74936289649118604</v>
       </c>
-      <c r="N11" s="1">
+      <c r="O12" s="1">
         <v>-7.52054972118604E-2</v>
       </c>
-      <c r="O11" s="1">
+      <c r="P12" s="1">
         <v>-4.1356771561809599E-2</v>
       </c>
-      <c r="P11" s="1">
+      <c r="Q12" s="1">
         <v>-0.33749619353839</v>
       </c>
-      <c r="Q11" s="1">
+      <c r="R12" s="1">
         <v>0.110375394470437</v>
       </c>
-      <c r="R11" s="1">
+      <c r="S12" s="1">
         <v>-0.26488931694418799</v>
       </c>
-      <c r="S11" s="1">
+      <c r="T12" s="1">
         <v>-0.242388645114026</v>
       </c>
-      <c r="T11" s="1">
+      <c r="U12" s="1">
         <v>0.205929940314552</v>
       </c>
-      <c r="U11" s="1">
+      <c r="V12" s="1">
         <v>0.19569739718309001</v>
       </c>
-      <c r="V11" s="1">
+      <c r="W12" s="1">
         <v>0.328722558060422</v>
       </c>
-      <c r="W11" s="1">
+      <c r="X12" s="1">
         <v>-9.7946995756107696E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:23">
-      <c r="A12" s="1" t="s">
+    <row r="13" spans="1:24">
+      <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B13" s="1">
         <v>-6.0427788055856302E-2</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C13" s="1">
         <v>-6.0414778618035798E-2</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D13" s="1">
+        <v>7.8799806840581191E-3</v>
+      </c>
+      <c r="E13" s="1">
         <v>-5.7796061324969901E-2</v>
       </c>
-      <c r="E12" s="1">
+      <c r="F13" s="1">
         <v>-1.89899379176257E-2</v>
       </c>
-      <c r="F12" s="1">
+      <c r="G13" s="1">
         <v>-6.2035063952588398E-2</v>
       </c>
-      <c r="G12" s="1">
+      <c r="H13" s="1">
         <v>-2.4345175331035199E-3</v>
       </c>
-      <c r="H12" s="1">
+      <c r="I13" s="1">
         <v>-4.5622654964447701E-2</v>
       </c>
-      <c r="I12" s="1">
+      <c r="J13" s="1">
         <v>-7.0223322368931806E-2</v>
       </c>
-      <c r="J12" s="1">
+      <c r="K13" s="1">
         <v>2.3054050853716999E-2</v>
       </c>
-      <c r="K12" s="1">
+      <c r="L13" s="1">
         <v>-7.2841808258598595E-2</v>
       </c>
-      <c r="L12" s="1">
-        <v>1</v>
-      </c>
-      <c r="M12" s="1">
+      <c r="M13" s="1">
+        <v>1</v>
+      </c>
+      <c r="N13" s="1">
         <v>-6.9654351468757703E-2</v>
       </c>
-      <c r="N12" s="1">
+      <c r="O13" s="1">
         <v>2.7036991980495501E-2</v>
       </c>
-      <c r="O12" s="1">
+      <c r="P13" s="1">
         <v>-1.6156580888312001E-2</v>
       </c>
-      <c r="P12" s="1">
+      <c r="Q13" s="1">
         <v>3.9904294529949799E-2</v>
       </c>
-      <c r="Q12" s="1">
+      <c r="R13" s="1">
         <v>-1.5323664056820899E-2</v>
       </c>
-      <c r="R12" s="1">
+      <c r="S13" s="1">
         <v>2.6052724833825699E-2</v>
       </c>
-      <c r="S12" s="1">
+      <c r="T13" s="1">
         <v>1.8019281951949701E-2</v>
       </c>
-      <c r="T12" s="1">
+      <c r="U13" s="1">
         <v>-1.93027494948791E-2</v>
       </c>
-      <c r="U12" s="1">
+      <c r="V13" s="1">
         <v>-2.92832271632666E-2</v>
       </c>
-      <c r="V12" s="1">
+      <c r="W13" s="1">
         <v>-4.4458415243685302E-2</v>
       </c>
-      <c r="W12" s="1">
+      <c r="X13" s="1">
         <v>-1.15433425578127E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:23">
-      <c r="A13" s="1" t="s">
+    <row r="14" spans="1:24">
+      <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B14" s="1">
         <v>0.82953931281323101</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C14" s="1">
         <v>0.82931677738246801</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D14" s="1">
+        <v>4.5054659352377797E-2</v>
+      </c>
+      <c r="E14" s="1">
         <v>0.824898287043488</v>
       </c>
-      <c r="E13" s="1">
+      <c r="F14" s="1">
         <v>0.37065066700242599</v>
       </c>
-      <c r="F13" s="1">
+      <c r="G14" s="1">
         <v>0.49834246183970299</v>
       </c>
-      <c r="G13" s="1">
+      <c r="H14" s="1">
         <v>-0.22966969875881099</v>
       </c>
-      <c r="H13" s="1">
+      <c r="I14" s="1">
         <v>0.716496238438313</v>
       </c>
-      <c r="I13" s="1">
+      <c r="J14" s="1">
         <v>0.68085225192023602</v>
       </c>
-      <c r="J13" s="1">
+      <c r="K14" s="1">
         <v>-0.10966046937912299</v>
       </c>
-      <c r="K13" s="1">
+      <c r="L14" s="1">
         <v>0.74936289649118604</v>
       </c>
-      <c r="L13" s="1">
+      <c r="M14" s="1">
         <v>-6.9654351468757703E-2</v>
       </c>
-      <c r="M13" s="1">
-        <v>1</v>
-      </c>
-      <c r="N13" s="1">
+      <c r="N14" s="1">
+        <v>1</v>
+      </c>
+      <c r="O14" s="1">
         <v>-6.14696002938026E-2</v>
       </c>
-      <c r="O13" s="1">
+      <c r="P14" s="1">
         <v>-2.33860824943329E-2</v>
       </c>
-      <c r="P13" s="1">
+      <c r="Q14" s="1">
         <v>-0.33724890447026101</v>
       </c>
-      <c r="Q13" s="1">
+      <c r="R14" s="1">
         <v>0.11965365328777</v>
       </c>
-      <c r="R13" s="1">
+      <c r="S14" s="1">
         <v>-0.28078491905499797</v>
       </c>
-      <c r="S13" s="1">
+      <c r="T14" s="1">
         <v>-0.25897274376178497</v>
       </c>
-      <c r="T13" s="1">
+      <c r="U14" s="1">
         <v>0.187633020878054</v>
       </c>
-      <c r="U13" s="1">
+      <c r="V14" s="1">
         <v>0.18395981514096901</v>
       </c>
-      <c r="V13" s="1">
+      <c r="W14" s="1">
         <v>0.32669137020422701</v>
       </c>
-      <c r="W13" s="1">
+      <c r="X14" s="1">
         <v>-8.0106668520529192E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:23">
-      <c r="A14" s="1" t="s">
+    <row r="15" spans="1:24">
+      <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B15" s="1">
         <v>-5.9284016850549598E-2</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C15" s="1">
         <v>-5.9246892135405203E-2</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D15" s="1">
+        <v>3.9442973294892504E-3</v>
+      </c>
+      <c r="E15" s="1">
         <v>-5.7649057638550202E-2</v>
       </c>
-      <c r="E14" s="1">
+      <c r="F15" s="1">
         <v>-1.9336857556304401E-2</v>
       </c>
-      <c r="F14" s="1">
+      <c r="G15" s="1">
         <v>-6.5784057174292601E-2</v>
       </c>
-      <c r="G14" s="1">
+      <c r="H15" s="1">
         <v>5.2996348825765302E-3</v>
       </c>
-      <c r="H14" s="1">
+      <c r="I15" s="1">
         <v>-4.4383525496576502E-2</v>
       </c>
-      <c r="I14" s="1">
+      <c r="J15" s="1">
         <v>-5.7117563177665198E-2</v>
       </c>
-      <c r="J14" s="1">
+      <c r="K15" s="1">
         <v>3.91858113923442E-2</v>
       </c>
-      <c r="K14" s="1">
+      <c r="L15" s="1">
         <v>-7.52054972118604E-2</v>
       </c>
-      <c r="L14" s="1">
+      <c r="M15" s="1">
         <v>2.7036991980495501E-2</v>
       </c>
-      <c r="M14" s="1">
+      <c r="N15" s="1">
         <v>-6.14696002938026E-2</v>
       </c>
-      <c r="N14" s="1">
-        <v>1</v>
-      </c>
-      <c r="O14" s="1">
+      <c r="O15" s="1">
+        <v>1</v>
+      </c>
+      <c r="P15" s="1">
         <v>-2.1889694913207199E-2</v>
       </c>
-      <c r="P14" s="1">
+      <c r="Q15" s="1">
         <v>4.4818181259573098E-2</v>
       </c>
-      <c r="Q14" s="1">
+      <c r="R15" s="1">
         <v>1.52081396592591E-3</v>
       </c>
-      <c r="R14" s="1">
+      <c r="S15" s="1">
         <v>2.05397840169072E-2</v>
       </c>
-      <c r="S14" s="1">
+      <c r="T15" s="1">
         <v>1.44049105906168E-2</v>
       </c>
-      <c r="T14" s="1">
+      <c r="U15" s="1">
         <v>-1.3836211561425799E-2</v>
       </c>
-      <c r="U14" s="1">
+      <c r="V15" s="1">
         <v>-1.9330756607418401E-2</v>
       </c>
-      <c r="V14" s="1">
+      <c r="W15" s="1">
         <v>-4.9886605917752701E-2</v>
       </c>
-      <c r="W14" s="1">
+      <c r="X15" s="1">
         <v>-5.04709052388767E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:23">
-      <c r="A15" s="1" t="s">
+    <row r="16" spans="1:24">
+      <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B16" s="1">
         <v>-6.4356048591548498E-3</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C16" s="1">
         <v>-6.4070399287441699E-3</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D16" s="1">
+        <v>2.9092633138568101E-2</v>
+      </c>
+      <c r="E16" s="1">
         <v>1.0192436571006399E-2</v>
       </c>
-      <c r="E15" s="1">
+      <c r="F16" s="1">
         <v>-2.4707453693601001E-3</v>
       </c>
-      <c r="F15" s="1">
+      <c r="G16" s="1">
         <v>2.6804991343021001E-2</v>
       </c>
-      <c r="G15" s="1">
+      <c r="H16" s="2">
         <v>0.27997741363661999</v>
       </c>
-      <c r="H15" s="1">
+      <c r="I16" s="1">
         <v>-0.137694814632288</v>
       </c>
-      <c r="I15" s="1">
+      <c r="J16" s="1">
         <v>-6.55828885203881E-2</v>
       </c>
-      <c r="J15" s="1">
+      <c r="K16" s="1">
         <v>-1.43555239103151E-2</v>
       </c>
-      <c r="K15" s="1">
+      <c r="L16" s="1">
         <v>-4.1356771561809599E-2</v>
       </c>
-      <c r="L15" s="1">
+      <c r="M16" s="1">
         <v>-1.6156580888312001E-2</v>
       </c>
-      <c r="M15" s="1">
+      <c r="N16" s="1">
         <v>-2.33860824943329E-2</v>
       </c>
-      <c r="N15" s="1">
+      <c r="O16" s="1">
         <v>-2.1889694913207199E-2</v>
       </c>
-      <c r="O15" s="1">
-        <v>1</v>
-      </c>
-      <c r="P15" s="1">
+      <c r="P16" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="2">
         <v>0.41658916643764898</v>
       </c>
-      <c r="Q15" s="1">
+      <c r="R16" s="2">
         <v>0.75222567222179804</v>
       </c>
-      <c r="R15" s="1">
+      <c r="S16" s="1">
         <v>5.1546238393481998E-2</v>
       </c>
-      <c r="S15" s="1">
+      <c r="T16" s="1">
         <v>4.5181059432952898E-2</v>
       </c>
-      <c r="T15" s="1">
+      <c r="U16" s="1">
         <v>0.120471124499507</v>
       </c>
-      <c r="U15" s="1">
+      <c r="V16" s="1">
         <v>9.0533357017126101E-2</v>
       </c>
-      <c r="V15" s="1">
+      <c r="W16" s="1">
         <v>0.177372877488015</v>
       </c>
-      <c r="W15" s="1">
+      <c r="X16" s="1">
         <v>5.9140067636493002E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:23">
-      <c r="A16" s="1" t="s">
+    <row r="17" spans="1:24">
+      <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B17" s="1">
         <v>-0.37757899773043102</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C17" s="1">
         <v>-0.37776479910271898</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D17" s="1">
+        <v>-5.89000038995382E-2</v>
+      </c>
+      <c r="E17" s="1">
         <v>-0.37222931181248903</v>
       </c>
-      <c r="E16" s="1">
+      <c r="F17" s="1">
         <v>-0.204306532318446</v>
       </c>
-      <c r="F16" s="1">
+      <c r="G17" s="1">
         <v>-0.25337149820265797</v>
       </c>
-      <c r="G16" s="1">
+      <c r="H17" s="1">
         <v>0.28744392203068803</v>
       </c>
-      <c r="H16" s="1">
+      <c r="I17" s="1">
         <v>-0.405744291142562</v>
       </c>
-      <c r="I16" s="1">
+      <c r="J17" s="1">
         <v>-0.32236566895984797</v>
       </c>
-      <c r="J16" s="1">
+      <c r="K17" s="1">
         <v>9.6562390623278302E-2</v>
       </c>
-      <c r="K16" s="1">
+      <c r="L17" s="1">
         <v>-0.33749619353839</v>
       </c>
-      <c r="L16" s="1">
+      <c r="M17" s="1">
         <v>3.9904294529949799E-2</v>
       </c>
-      <c r="M16" s="1">
+      <c r="N17" s="1">
         <v>-0.33724890447026101</v>
       </c>
-      <c r="N16" s="1">
+      <c r="O17" s="1">
         <v>4.4818181259573098E-2</v>
       </c>
-      <c r="O16" s="1">
+      <c r="P17" s="1">
         <v>0.41658916643764898</v>
       </c>
-      <c r="P16" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q16" s="1">
+      <c r="Q17" s="1">
+        <v>1</v>
+      </c>
+      <c r="R17" s="1">
         <v>0.33380468449307898</v>
       </c>
-      <c r="R16" s="1">
+      <c r="S17" s="1">
         <v>0.19784953544106099</v>
       </c>
-      <c r="S16" s="1">
+      <c r="T17" s="1">
         <v>0.17684953017551899</v>
       </c>
-      <c r="T16" s="1">
+      <c r="U17" s="1">
         <v>-6.0553217759763703E-2</v>
       </c>
-      <c r="U16" s="1">
+      <c r="V17" s="1">
         <v>-8.9276154852037201E-2</v>
       </c>
-      <c r="V16" s="1">
+      <c r="W17" s="1">
         <v>-0.103480981711129</v>
       </c>
-      <c r="W16" s="1">
+      <c r="X17" s="1">
         <v>-1.38183675263011E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:23">
-      <c r="A17" s="1" t="s">
+    <row r="18" spans="1:24">
+      <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B18" s="1">
         <v>0.13964079269922999</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C18" s="1">
         <v>0.140383475580452</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D18" s="1">
+        <v>4.2543278785014897E-2</v>
+      </c>
+      <c r="E18" s="1">
         <v>0.14443773167414201</v>
       </c>
-      <c r="E17" s="1">
+      <c r="F18" s="1">
         <v>7.6023292156156302E-2</v>
       </c>
-      <c r="F17" s="1">
+      <c r="G18" s="1">
         <v>8.8547129555941795E-2</v>
       </c>
-      <c r="G17" s="1">
+      <c r="H18" s="1">
         <v>0.26762153705583802</v>
       </c>
-      <c r="H17" s="1">
+      <c r="I18" s="1">
         <v>-1.5969107993542501E-3</v>
       </c>
-      <c r="I17" s="1">
+      <c r="J18" s="1">
         <v>7.5053026801822603E-2</v>
       </c>
-      <c r="J17" s="1">
+      <c r="K18" s="1">
         <v>-1.8039308090925001E-2</v>
       </c>
-      <c r="K17" s="1">
+      <c r="L18" s="1">
         <v>0.110375394470437</v>
       </c>
-      <c r="L17" s="1">
+      <c r="M18" s="1">
         <v>-1.5323664056820899E-2</v>
       </c>
-      <c r="M17" s="1">
+      <c r="N18" s="1">
         <v>0.11965365328777</v>
       </c>
-      <c r="N17" s="1">
+      <c r="O18" s="1">
         <v>1.52081396592591E-3</v>
       </c>
-      <c r="O17" s="1">
+      <c r="P18" s="1">
         <v>0.75222567222179804</v>
       </c>
-      <c r="P17" s="1">
+      <c r="Q18" s="1">
         <v>0.33380468449307898</v>
       </c>
-      <c r="Q17" s="1">
-        <v>1</v>
-      </c>
-      <c r="R17" s="1">
+      <c r="R18" s="1">
+        <v>1</v>
+      </c>
+      <c r="S18" s="1">
         <v>3.6453453802751598E-2</v>
       </c>
-      <c r="S17" s="1">
+      <c r="T18" s="1">
         <v>3.8208184834743197E-2</v>
       </c>
-      <c r="T17" s="1">
+      <c r="U18" s="1">
         <v>0.162490306128941</v>
       </c>
-      <c r="U17" s="1">
+      <c r="V18" s="1">
         <v>0.12704038399133899</v>
       </c>
-      <c r="V17" s="1">
+      <c r="W18" s="1">
         <v>0.19241623078237099</v>
       </c>
-      <c r="W17" s="1">
+      <c r="X18" s="1">
         <v>-1.11525015845945E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:23">
-      <c r="A18" s="1" t="s">
+    <row r="19" spans="1:24">
+      <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B19" s="1">
         <v>-0.35900228946907298</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C19" s="1">
         <v>-0.35147626159824102</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D19" s="1">
+        <v>-3.4044314085956297E-2</v>
+      </c>
+      <c r="E19" s="1">
         <v>-0.34969712063187403</v>
       </c>
-      <c r="E18" s="1">
+      <c r="F19" s="1">
         <v>-0.160096799255316</v>
       </c>
-      <c r="F18" s="1">
+      <c r="G19" s="1">
         <v>-0.25328117586416798</v>
       </c>
-      <c r="G18" s="1">
+      <c r="H19" s="1">
         <v>0.17959151254904701</v>
       </c>
-      <c r="H18" s="1">
+      <c r="I19" s="1">
         <v>-0.25764650010722501</v>
       </c>
-      <c r="I18" s="1">
+      <c r="J19" s="1">
         <v>-0.19581622016279601</v>
       </c>
-      <c r="J18" s="1">
+      <c r="K19" s="1">
         <v>4.3301105885510199E-2</v>
       </c>
-      <c r="K18" s="1">
+      <c r="L19" s="1">
         <v>-0.26488931694418799</v>
       </c>
-      <c r="L18" s="1">
+      <c r="M19" s="1">
         <v>2.6052724833825699E-2</v>
       </c>
-      <c r="M18" s="1">
+      <c r="N19" s="1">
         <v>-0.28078491905499797</v>
       </c>
-      <c r="N18" s="1">
+      <c r="O19" s="1">
         <v>2.05397840169072E-2</v>
       </c>
-      <c r="O18" s="1">
+      <c r="P19" s="1">
         <v>5.1546238393481998E-2</v>
       </c>
-      <c r="P18" s="1">
+      <c r="Q19" s="1">
         <v>0.19784953544106099</v>
       </c>
-      <c r="Q18" s="1">
+      <c r="R19" s="1">
         <v>3.6453453802751598E-2</v>
       </c>
-      <c r="R18" s="1">
-        <v>1</v>
-      </c>
-      <c r="S18" s="1">
-        <v>1</v>
-      </c>
-      <c r="T18" s="1">
+      <c r="S19" s="1">
+        <v>1</v>
+      </c>
+      <c r="T19" s="1">
+        <v>1</v>
+      </c>
+      <c r="U19" s="1">
         <v>8.5290818743362404E-2</v>
       </c>
-      <c r="U18" s="1">
+      <c r="V19" s="1">
         <v>3.4882645304199898E-2</v>
       </c>
-      <c r="V18" s="1">
+      <c r="W19" s="1">
         <v>-0.14889165209272601</v>
       </c>
-      <c r="W18" s="1">
+      <c r="X19" s="1">
         <v>2.3871610716710699E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:23">
-      <c r="A19" s="1" t="s">
+    <row r="20" spans="1:24">
+      <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B20" s="1">
         <v>-0.33986937510027498</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C20" s="1">
         <v>-0.33121623145919099</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D20" s="1">
+        <v>-4.0034757956118897E-2</v>
+      </c>
+      <c r="E20" s="1">
         <v>-0.33126226376010198</v>
       </c>
-      <c r="E19" s="1">
+      <c r="F20" s="1">
         <v>-0.153085545779267</v>
       </c>
-      <c r="F19" s="1">
+      <c r="G20" s="1">
         <v>-0.23454979796974099</v>
       </c>
-      <c r="G19" s="1">
+      <c r="H20" s="1">
         <v>0.17529322024326099</v>
       </c>
-      <c r="H19" s="1">
+      <c r="I20" s="1">
         <v>-0.232515081609737</v>
       </c>
-      <c r="I19" s="1">
+      <c r="J20" s="1">
         <v>-0.163888398594911</v>
       </c>
-      <c r="J19" s="1">
+      <c r="K20" s="1">
         <v>3.1900159353646297E-2</v>
       </c>
-      <c r="K19" s="1">
+      <c r="L20" s="1">
         <v>-0.242388645114026</v>
       </c>
-      <c r="L19" s="1">
+      <c r="M20" s="1">
         <v>1.8019281951949701E-2</v>
       </c>
-      <c r="M19" s="1">
+      <c r="N20" s="1">
         <v>-0.25897274376178497</v>
       </c>
-      <c r="N19" s="1">
+      <c r="O20" s="1">
         <v>1.44049105906168E-2</v>
       </c>
-      <c r="O19" s="1">
+      <c r="P20" s="1">
         <v>4.5181059432952898E-2</v>
       </c>
-      <c r="P19" s="1">
+      <c r="Q20" s="1">
         <v>0.17684953017551899</v>
       </c>
-      <c r="Q19" s="1">
+      <c r="R20" s="1">
         <v>3.8208184834743197E-2</v>
       </c>
-      <c r="R19" s="1">
-        <v>1</v>
-      </c>
-      <c r="S19" s="1">
-        <v>1</v>
-      </c>
-      <c r="T19" s="1">
+      <c r="S20" s="1">
+        <v>1</v>
+      </c>
+      <c r="T20" s="1">
+        <v>1</v>
+      </c>
+      <c r="U20" s="1">
         <v>0.11006620190765</v>
       </c>
-      <c r="U19" s="1">
+      <c r="V20" s="1">
         <v>6.0408894316445201E-2</v>
       </c>
-      <c r="V19" s="1">
+      <c r="W20" s="1">
         <v>-0.13493336284254101</v>
       </c>
-      <c r="W19" s="1">
+      <c r="X20" s="1">
         <v>8.0165314112054201E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:23">
-      <c r="A20" s="1" t="s">
+    <row r="21" spans="1:24">
+      <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B21" s="1">
         <v>0.158547389500029</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C21" s="1">
         <v>0.160128190714033</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D21" s="1">
+        <v>1.1101529625722599E-2</v>
+      </c>
+      <c r="E21" s="1">
         <v>0.15579318259889099</v>
       </c>
-      <c r="E20" s="1">
+      <c r="F21" s="1">
         <v>5.4749769816534698E-2</v>
       </c>
-      <c r="F20" s="1">
+      <c r="G21" s="1">
         <v>9.78272645040488E-2</v>
       </c>
-      <c r="G20" s="1">
+      <c r="H21" s="1">
         <v>8.2227941978073801E-2</v>
       </c>
-      <c r="H20" s="1">
+      <c r="I21" s="1">
         <v>0.159663790236064</v>
       </c>
-      <c r="I20" s="1">
+      <c r="J21" s="1">
         <v>0.221129605573503</v>
       </c>
-      <c r="J20" s="1">
+      <c r="K21" s="1">
         <v>-2.88341948922398E-2</v>
       </c>
-      <c r="K20" s="1">
+      <c r="L21" s="1">
         <v>0.205929940314552</v>
       </c>
-      <c r="L20" s="1">
+      <c r="M21" s="1">
         <v>-1.93027494948791E-2</v>
       </c>
-      <c r="M20" s="1">
+      <c r="N21" s="1">
         <v>0.187633020878054</v>
       </c>
-      <c r="N20" s="1">
+      <c r="O21" s="1">
         <v>-1.3836211561425799E-2</v>
       </c>
-      <c r="O20" s="1">
+      <c r="P21" s="1">
         <v>0.120471124499507</v>
       </c>
-      <c r="P20" s="1">
+      <c r="Q21" s="1">
         <v>-6.0553217759763703E-2</v>
       </c>
-      <c r="Q20" s="1">
+      <c r="R21" s="1">
         <v>0.162490306128941</v>
       </c>
-      <c r="R20" s="1">
+      <c r="S21" s="1">
         <v>8.5290818743362404E-2</v>
       </c>
-      <c r="S20" s="1">
+      <c r="T21" s="1">
         <v>0.11006620190765</v>
       </c>
-      <c r="T20" s="1">
-        <v>1</v>
-      </c>
-      <c r="U20" s="1">
+      <c r="U21" s="1">
+        <v>1</v>
+      </c>
+      <c r="V21" s="1">
         <v>0.59644998969615803</v>
       </c>
-      <c r="V20" s="1">
+      <c r="W21" s="1">
         <v>8.4078869037076703E-2</v>
       </c>
-      <c r="W20" s="1">
+      <c r="X21" s="1">
         <v>-7.3597104029237302E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:23">
-      <c r="A21" s="1" t="s">
+    <row r="22" spans="1:24">
+      <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B22" s="1">
         <v>0.15663073697514199</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C22" s="1">
         <v>0.15765222565210299</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D22" s="1">
+        <v>-1.8688684323293701E-2</v>
+      </c>
+      <c r="E22" s="1">
         <v>0.15176570459345301</v>
       </c>
-      <c r="E21" s="1">
+      <c r="F22" s="1">
         <v>4.26502746904645E-2</v>
       </c>
-      <c r="F21" s="1">
+      <c r="G22" s="1">
         <v>9.66665551086099E-2</v>
       </c>
-      <c r="G21" s="1">
+      <c r="H22" s="1">
         <v>7.0725267050235796E-2</v>
       </c>
-      <c r="H21" s="1">
+      <c r="I22" s="1">
         <v>0.180142957024571</v>
       </c>
-      <c r="I21" s="1">
+      <c r="J22" s="1">
         <v>0.20519369984307501</v>
       </c>
-      <c r="J21" s="1">
+      <c r="K22" s="1">
         <v>-3.2350507379077902E-2</v>
       </c>
-      <c r="K21" s="1">
+      <c r="L22" s="1">
         <v>0.19569739718309001</v>
       </c>
-      <c r="L21" s="1">
+      <c r="M22" s="1">
         <v>-2.92832271632666E-2</v>
       </c>
-      <c r="M21" s="1">
+      <c r="N22" s="1">
         <v>0.18395981514096901</v>
       </c>
-      <c r="N21" s="1">
+      <c r="O22" s="1">
         <v>-1.9330756607418401E-2</v>
       </c>
-      <c r="O21" s="1">
+      <c r="P22" s="1">
         <v>9.0533357017126101E-2</v>
       </c>
-      <c r="P21" s="1">
+      <c r="Q22" s="1">
         <v>-8.9276154852037201E-2</v>
       </c>
-      <c r="Q21" s="1">
+      <c r="R22" s="1">
         <v>0.12704038399133899</v>
       </c>
-      <c r="R21" s="1">
+      <c r="S22" s="1">
         <v>3.4882645304199898E-2</v>
       </c>
-      <c r="S21" s="1">
+      <c r="T22" s="1">
         <v>6.0408894316445201E-2</v>
       </c>
-      <c r="T21" s="1">
+      <c r="U22" s="1">
         <v>0.59644998969615803</v>
       </c>
-      <c r="U21" s="1">
-        <v>1</v>
-      </c>
-      <c r="V21" s="1">
+      <c r="V22" s="1">
+        <v>1</v>
+      </c>
+      <c r="W22" s="1">
         <v>9.6275308008923102E-2</v>
       </c>
-      <c r="W21" s="1">
+      <c r="X22" s="1">
         <v>2.8844202110653101E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:23">
-      <c r="A22" s="1" t="s">
+    <row r="23" spans="1:24">
+      <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B23" s="1">
         <v>0.36082637349743701</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C23" s="1">
         <v>0.36076580547304299</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D23" s="1">
+        <v>-7.9142521001483706E-3</v>
+      </c>
+      <c r="E23" s="1">
         <v>0.36388318087433702</v>
       </c>
-      <c r="E22" s="1">
+      <c r="F23" s="1">
         <v>0.167463118225393</v>
       </c>
-      <c r="F22" s="1">
+      <c r="G23" s="1">
         <v>0.35248858014956302</v>
       </c>
-      <c r="G22" s="1">
+      <c r="H23" s="1">
         <v>-4.9181399633654699E-2</v>
       </c>
-      <c r="H22" s="1">
+      <c r="I23" s="1">
         <v>0.30193287043511802</v>
       </c>
-      <c r="I22" s="1">
+      <c r="J23" s="1">
         <v>0.30519050901529099</v>
       </c>
-      <c r="J22" s="1">
+      <c r="K23" s="1">
         <v>-5.7516400188989097E-2</v>
       </c>
-      <c r="K22" s="1">
+      <c r="L23" s="1">
         <v>0.328722558060422</v>
       </c>
-      <c r="L22" s="1">
+      <c r="M23" s="1">
         <v>-4.4458415243685302E-2</v>
       </c>
-      <c r="M22" s="1">
+      <c r="N23" s="1">
         <v>0.32669137020422701</v>
       </c>
-      <c r="N22" s="1">
+      <c r="O23" s="1">
         <v>-4.9886605917752701E-2</v>
       </c>
-      <c r="O22" s="1">
+      <c r="P23" s="1">
         <v>0.177372877488015</v>
       </c>
-      <c r="P22" s="1">
+      <c r="Q23" s="1">
         <v>-0.103480981711129</v>
       </c>
-      <c r="Q22" s="1">
+      <c r="R23" s="1">
         <v>0.19241623078237099</v>
       </c>
-      <c r="R22" s="1">
+      <c r="S23" s="1">
         <v>-0.14889165209272601</v>
       </c>
-      <c r="S22" s="1">
+      <c r="T23" s="1">
         <v>-0.13493336284254101</v>
       </c>
-      <c r="T22" s="1">
+      <c r="U23" s="1">
         <v>8.4078869037076703E-2</v>
       </c>
-      <c r="U22" s="1">
+      <c r="V23" s="1">
         <v>9.6275308008923102E-2</v>
       </c>
-      <c r="V22" s="1">
-        <v>1</v>
-      </c>
-      <c r="W22" s="1">
+      <c r="W23" s="1">
+        <v>1</v>
+      </c>
+      <c r="X23" s="1">
         <v>7.7809115904854606E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:23">
-      <c r="A23" s="1" t="s">
+    <row r="24" spans="1:24">
+      <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B24" s="1">
         <v>-1.38913900613486E-2</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C24" s="1">
         <v>-1.34636929694276E-2</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D24" s="1">
+        <v>-7.0963342595646199E-3</v>
+      </c>
+      <c r="E24" s="1">
         <v>-2.48133817072945E-2</v>
       </c>
-      <c r="E23" s="1">
+      <c r="F24" s="1">
         <v>-2.80160139628737E-2</v>
       </c>
-      <c r="F23" s="1">
+      <c r="G24" s="1">
         <v>1.27596430203949E-2</v>
       </c>
-      <c r="G23" s="1">
+      <c r="H24" s="1">
         <v>-0.11376401354828899</v>
       </c>
-      <c r="H23" s="1">
+      <c r="I24" s="1">
         <v>1.15459971934405E-2</v>
       </c>
-      <c r="I23" s="1">
+      <c r="J24" s="1">
         <v>1.91520432036506E-2</v>
       </c>
-      <c r="J23" s="1">
+      <c r="K24" s="1">
         <v>-1.39286712044361E-2</v>
       </c>
-      <c r="K23" s="1">
+      <c r="L24" s="1">
         <v>-9.7946995756107696E-3</v>
       </c>
-      <c r="L23" s="1">
+      <c r="M24" s="1">
         <v>-1.15433425578127E-2</v>
       </c>
-      <c r="M23" s="1">
+      <c r="N24" s="1">
         <v>-8.0106668520529192E-3</v>
       </c>
-      <c r="N23" s="1">
+      <c r="O24" s="1">
         <v>-5.04709052388767E-3</v>
       </c>
-      <c r="O23" s="1">
+      <c r="P24" s="1">
         <v>5.9140067636493002E-2</v>
       </c>
-      <c r="P23" s="1">
+      <c r="Q24" s="1">
         <v>-1.38183675263011E-2</v>
       </c>
-      <c r="Q23" s="1">
+      <c r="R24" s="1">
         <v>-1.11525015845945E-2</v>
       </c>
-      <c r="R23" s="1">
+      <c r="S24" s="1">
         <v>2.3871610716710699E-2</v>
       </c>
-      <c r="S23" s="1">
+      <c r="T24" s="1">
         <v>8.0165314112054201E-2</v>
       </c>
-      <c r="T23" s="1">
+      <c r="U24" s="1">
         <v>-7.3597104029237302E-3</v>
       </c>
-      <c r="U23" s="1">
+      <c r="V24" s="1">
         <v>2.8844202110653101E-2</v>
       </c>
-      <c r="V23" s="1">
+      <c r="W24" s="1">
         <v>7.7809115904854606E-2</v>
       </c>
-      <c r="W23" s="1">
+      <c r="X24" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>